<commit_message>
Resolved encapsulation issues in file manager. Name mangling
</commit_message>
<xml_diff>
--- a/test_database/tester_database.xlsx
+++ b/test_database/tester_database.xlsx
@@ -532,7 +532,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C101"/>
+  <dimension ref="A1:C102"/>
   <sheetViews>
     <sheetView topLeftCell="A47" workbookViewId="0">
       <selection activeCell="C90" sqref="C90:C99"/>
@@ -2061,6 +2061,21 @@
         <v>9</v>
       </c>
     </row>
+    <row r="102">
+      <c r="A102" t="inlineStr">
+        <is>
+          <t>socks</t>
+        </is>
+      </c>
+      <c r="B102" t="inlineStr">
+        <is>
+          <t>skarpety</t>
+        </is>
+      </c>
+      <c r="C102" t="n">
+        <v>10</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2072,7 +2087,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B10"/>
+  <dimension ref="A1:B11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="D8" sqref="D8"/>
@@ -2185,6 +2200,16 @@
         </is>
       </c>
     </row>
+    <row r="11">
+      <c r="A11" t="n">
+        <v>10</v>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>Test level a1</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2196,7 +2221,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I11"/>
+  <dimension ref="A1:I13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="K3" sqref="K3"/>
@@ -2652,10 +2677,8 @@
       <c r="E11" t="n">
         <v>660</v>
       </c>
-      <c r="F11" t="inlineStr">
-        <is>
-          <t>73.46</t>
-        </is>
+      <c r="F11" t="n">
+        <v>73.45999999999999</v>
       </c>
       <c r="G11" t="inlineStr">
         <is>
@@ -2670,6 +2693,90 @@
       <c r="I11" t="inlineStr">
         <is>
           <t>Processors</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="n">
+        <v>11</v>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>Gienek</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>18-01-2025 01:32:58</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>EN-&gt;PL</t>
+        </is>
+      </c>
+      <c r="E12" t="n">
+        <v>60</v>
+      </c>
+      <c r="F12" t="n">
+        <v>6.75</v>
+      </c>
+      <c r="G12" t="inlineStr">
+        <is>
+          <t>(0/&lt;bound method NewTest.__get_questions_amount of &lt;test.test.NewTest object at 0x104d88980&gt;&gt;)</t>
+        </is>
+      </c>
+      <c r="H12" t="inlineStr">
+        <is>
+          <t>0.00%</t>
+        </is>
+      </c>
+      <c r="I12" t="inlineStr">
+        <is>
+          <t>Monitory, Keyboard, Test level a1</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="n">
+        <v>12</v>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>GIenek</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>18-01-2025 01:37:01</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>EN-&gt;PL</t>
+        </is>
+      </c>
+      <c r="E13" t="n">
+        <v>60</v>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>7.67</t>
+        </is>
+      </c>
+      <c r="G13" t="inlineStr">
+        <is>
+          <t>(1/&lt;bound method NewTest.__get_questions_amount of &lt;test.test.NewTest object at 0x105224830&gt;&gt;)</t>
+        </is>
+      </c>
+      <c r="H13" t="inlineStr">
+        <is>
+          <t>100.00%</t>
+        </is>
+      </c>
+      <c r="I13" t="inlineStr">
+        <is>
+          <t>Monitory, Keyboard, Test level a1</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Moved result analyzys from NewTest to ResultManager, solved encapsulation issues.
</commit_message>
<xml_diff>
--- a/test_database/tester_database.xlsx
+++ b/test_database/tester_database.xlsx
@@ -2221,7 +2221,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I13"/>
+  <dimension ref="A1:I14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="K3" sqref="K3"/>
@@ -2759,10 +2759,8 @@
       <c r="E13" t="n">
         <v>60</v>
       </c>
-      <c r="F13" t="inlineStr">
-        <is>
-          <t>7.67</t>
-        </is>
+      <c r="F13" t="n">
+        <v>7.67</v>
       </c>
       <c r="G13" t="inlineStr">
         <is>
@@ -2777,6 +2775,49 @@
       <c r="I13" t="inlineStr">
         <is>
           <t>Monitory, Keyboard, Test level a1</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="n">
+        <v>13</v>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>asdfasf</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>19-01-202500:00:53</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>EN-&gt;PL</t>
+        </is>
+      </c>
+      <c r="E14" t="n">
+        <v>240</v>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>10.74</t>
+        </is>
+      </c>
+      <c r="G14" t="inlineStr">
+        <is>
+          <t>(2/None)</t>
+        </is>
+      </c>
+      <c r="H14" t="inlineStr">
+        <is>
+          <t>50.00%</t>
+        </is>
+      </c>
+      <c r="I14" t="inlineStr">
+        <is>
+          <t>Games Remastering</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Added questions numeration during test
</commit_message>
<xml_diff>
--- a/test_database/tester_database.xlsx
+++ b/test_database/tester_database.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="0" yWindow="0" windowWidth="38400" windowHeight="21600" tabRatio="600" firstSheet="0" activeTab="1" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="0" yWindow="500" windowWidth="38400" windowHeight="19700" tabRatio="600" firstSheet="0" activeTab="2" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="vocabluary" sheetId="1" state="visible" r:id="rId1"/>
@@ -49,11 +49,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <name val="Aptos Narrow"/>
-      <b val="1"/>
-      <sz val="12"/>
-    </font>
-    <font>
       <name val="Arial"/>
       <family val="2"/>
       <color theme="1"/>
@@ -70,6 +65,11 @@
       <family val="1"/>
       <color theme="1"/>
       <sz val="11"/>
+    </font>
+    <font>
+      <name val="Aptos Narrow"/>
+      <b val="1"/>
+      <sz val="12"/>
     </font>
     <font>
       <b val="1"/>
@@ -122,15 +122,15 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="top"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
@@ -545,17 +545,17 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="9" t="inlineStr">
+      <c r="A1" s="8" t="inlineStr">
         <is>
           <t>EN</t>
         </is>
       </c>
-      <c r="B1" s="9" t="inlineStr">
+      <c r="B1" s="8" t="inlineStr">
         <is>
           <t>PL</t>
         </is>
       </c>
-      <c r="C1" s="9" t="inlineStr">
+      <c r="C1" s="8" t="inlineStr">
         <is>
           <t>category</t>
         </is>
@@ -1882,12 +1882,12 @@
       </c>
     </row>
     <row r="90">
-      <c r="A90" s="6" t="inlineStr">
+      <c r="A90" s="5" t="inlineStr">
         <is>
           <t>capital gains</t>
         </is>
       </c>
-      <c r="B90" s="7" t="inlineStr">
+      <c r="B90" s="6" t="inlineStr">
         <is>
           <t>zyski kapitałowe</t>
         </is>
@@ -1897,12 +1897,12 @@
       </c>
     </row>
     <row r="91">
-      <c r="A91" s="6" t="inlineStr">
+      <c r="A91" s="5" t="inlineStr">
         <is>
           <t>income tax</t>
         </is>
       </c>
-      <c r="B91" s="7" t="inlineStr">
+      <c r="B91" s="6" t="inlineStr">
         <is>
           <t>podatek dochodowy</t>
         </is>
@@ -1912,12 +1912,12 @@
       </c>
     </row>
     <row r="92">
-      <c r="A92" s="6" t="inlineStr">
+      <c r="A92" s="5" t="inlineStr">
         <is>
           <t>withholding</t>
         </is>
       </c>
-      <c r="B92" s="8" t="inlineStr">
+      <c r="B92" s="7" t="inlineStr">
         <is>
           <t>pobranie podatku z pensji</t>
         </is>
@@ -1927,12 +1927,12 @@
       </c>
     </row>
     <row r="93">
-      <c r="A93" s="6" t="inlineStr">
+      <c r="A93" s="5" t="inlineStr">
         <is>
           <t>revenue</t>
         </is>
       </c>
-      <c r="B93" s="8" t="inlineStr">
+      <c r="B93" s="7" t="inlineStr">
         <is>
           <t>przychód</t>
         </is>
@@ -1942,12 +1942,12 @@
       </c>
     </row>
     <row r="94">
-      <c r="A94" s="6" t="inlineStr">
+      <c r="A94" s="5" t="inlineStr">
         <is>
           <t>disbursements</t>
         </is>
       </c>
-      <c r="B94" s="8" t="inlineStr">
+      <c r="B94" s="7" t="inlineStr">
         <is>
           <t>wydatki</t>
         </is>
@@ -1957,12 +1957,12 @@
       </c>
     </row>
     <row r="95">
-      <c r="A95" s="6" t="inlineStr">
+      <c r="A95" s="5" t="inlineStr">
         <is>
           <t>gross income</t>
         </is>
       </c>
-      <c r="B95" s="8" t="inlineStr">
+      <c r="B95" s="7" t="inlineStr">
         <is>
           <t>dochód brutto</t>
         </is>
@@ -1972,12 +1972,12 @@
       </c>
     </row>
     <row r="96">
-      <c r="A96" s="6" t="inlineStr">
+      <c r="A96" s="5" t="inlineStr">
         <is>
           <t>net income</t>
         </is>
       </c>
-      <c r="B96" s="8" t="inlineStr">
+      <c r="B96" s="7" t="inlineStr">
         <is>
           <t>dochód netto</t>
         </is>
@@ -1987,12 +1987,12 @@
       </c>
     </row>
     <row r="97">
-      <c r="A97" s="6" t="inlineStr">
+      <c r="A97" s="5" t="inlineStr">
         <is>
           <t>compound interest</t>
         </is>
       </c>
-      <c r="B97" s="8" t="inlineStr">
+      <c r="B97" s="7" t="inlineStr">
         <is>
           <t>odsetki składane</t>
         </is>
@@ -2002,12 +2002,12 @@
       </c>
     </row>
     <row r="98">
-      <c r="A98" s="6" t="inlineStr">
+      <c r="A98" s="5" t="inlineStr">
         <is>
           <t>mortgage</t>
         </is>
       </c>
-      <c r="B98" s="8" t="inlineStr">
+      <c r="B98" s="7" t="inlineStr">
         <is>
           <t>hipoteka</t>
         </is>
@@ -2017,12 +2017,12 @@
       </c>
     </row>
     <row r="99">
-      <c r="A99" s="6" t="inlineStr">
+      <c r="A99" s="5" t="inlineStr">
         <is>
           <t>interest rate</t>
         </is>
       </c>
-      <c r="B99" s="8" t="inlineStr">
+      <c r="B99" s="7" t="inlineStr">
         <is>
           <t>stopa procentowa</t>
         </is>
@@ -2089,8 +2089,8 @@
   </sheetPr>
   <dimension ref="A1:B11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -2099,12 +2099,12 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="9" t="inlineStr">
+      <c r="A1" s="8" t="inlineStr">
         <is>
           <t>category_id</t>
         </is>
       </c>
-      <c r="B1" s="9" t="inlineStr">
+      <c r="B1" s="8" t="inlineStr">
         <is>
           <t>category_name</t>
         </is>
@@ -2221,10 +2221,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I14"/>
+  <dimension ref="A1:I11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K3" sqref="K3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G23" sqref="G23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16"/>
@@ -2661,12 +2661,12 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>7hn</t>
+          <t>Hitler</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>15-01-2025 13:27:07</t>
+          <t>19-01-202500:31:50</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
@@ -2675,149 +2675,26 @@
         </is>
       </c>
       <c r="E11" t="n">
-        <v>660</v>
-      </c>
-      <c r="F11" t="n">
-        <v>73.45999999999999</v>
+        <v>60</v>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>257.32</t>
+        </is>
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>(0/10)</t>
+          <t>(1/6)</t>
         </is>
       </c>
       <c r="H11" t="inlineStr">
         <is>
-          <t>0.00%</t>
+          <t>16.67%</t>
         </is>
       </c>
       <c r="I11" t="inlineStr">
         <is>
           <t>Processors</t>
-        </is>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="n">
-        <v>11</v>
-      </c>
-      <c r="B12" t="inlineStr">
-        <is>
-          <t>Gienek</t>
-        </is>
-      </c>
-      <c r="C12" t="inlineStr">
-        <is>
-          <t>18-01-2025 01:32:58</t>
-        </is>
-      </c>
-      <c r="D12" t="inlineStr">
-        <is>
-          <t>EN-&gt;PL</t>
-        </is>
-      </c>
-      <c r="E12" t="n">
-        <v>60</v>
-      </c>
-      <c r="F12" t="n">
-        <v>6.75</v>
-      </c>
-      <c r="G12" t="inlineStr">
-        <is>
-          <t>(0/&lt;bound method NewTest.__get_questions_amount of &lt;test.test.NewTest object at 0x104d88980&gt;&gt;)</t>
-        </is>
-      </c>
-      <c r="H12" t="inlineStr">
-        <is>
-          <t>0.00%</t>
-        </is>
-      </c>
-      <c r="I12" t="inlineStr">
-        <is>
-          <t>Monitory, Keyboard, Test level a1</t>
-        </is>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="n">
-        <v>12</v>
-      </c>
-      <c r="B13" t="inlineStr">
-        <is>
-          <t>GIenek</t>
-        </is>
-      </c>
-      <c r="C13" t="inlineStr">
-        <is>
-          <t>18-01-2025 01:37:01</t>
-        </is>
-      </c>
-      <c r="D13" t="inlineStr">
-        <is>
-          <t>EN-&gt;PL</t>
-        </is>
-      </c>
-      <c r="E13" t="n">
-        <v>60</v>
-      </c>
-      <c r="F13" t="n">
-        <v>7.67</v>
-      </c>
-      <c r="G13" t="inlineStr">
-        <is>
-          <t>(1/&lt;bound method NewTest.__get_questions_amount of &lt;test.test.NewTest object at 0x105224830&gt;&gt;)</t>
-        </is>
-      </c>
-      <c r="H13" t="inlineStr">
-        <is>
-          <t>100.00%</t>
-        </is>
-      </c>
-      <c r="I13" t="inlineStr">
-        <is>
-          <t>Monitory, Keyboard, Test level a1</t>
-        </is>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="n">
-        <v>13</v>
-      </c>
-      <c r="B14" t="inlineStr">
-        <is>
-          <t>asdfasf</t>
-        </is>
-      </c>
-      <c r="C14" t="inlineStr">
-        <is>
-          <t>19-01-202500:00:53</t>
-        </is>
-      </c>
-      <c r="D14" t="inlineStr">
-        <is>
-          <t>EN-&gt;PL</t>
-        </is>
-      </c>
-      <c r="E14" t="n">
-        <v>240</v>
-      </c>
-      <c r="F14" t="inlineStr">
-        <is>
-          <t>10.74</t>
-        </is>
-      </c>
-      <c r="G14" t="inlineStr">
-        <is>
-          <t>(2/None)</t>
-        </is>
-      </c>
-      <c r="H14" t="inlineStr">
-        <is>
-          <t>50.00%</t>
-        </is>
-      </c>
-      <c r="I14" t="inlineStr">
-        <is>
-          <t>Games Remastering</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
fixed typo in comment
</commit_message>
<xml_diff>
--- a/test_database/tester_database.xlsx
+++ b/test_database/tester_database.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="0" yWindow="500" windowWidth="38400" windowHeight="19700" tabRatio="600" firstSheet="0" activeTab="2" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="0" yWindow="500" windowWidth="34200" windowHeight="19700" tabRatio="600" firstSheet="0" activeTab="2" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="vocabluary" sheetId="1" state="visible" r:id="rId1"/>
@@ -18,7 +18,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="10">
+  <fonts count="11">
     <font>
       <name val="Aptos Narrow"/>
       <charset val="238"/>
@@ -72,6 +72,11 @@
       <sz val="12"/>
     </font>
     <font>
+      <name val="Aptos Narrow"/>
+      <b val="1"/>
+      <sz val="12"/>
+    </font>
+    <font>
       <b val="1"/>
     </font>
   </fonts>
@@ -83,12 +88,27 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="4">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -116,7 +136,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
@@ -133,6 +153,9 @@
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
@@ -534,7 +557,7 @@
   </sheetPr>
   <dimension ref="A1:C102"/>
   <sheetViews>
-    <sheetView topLeftCell="A47" workbookViewId="0">
+    <sheetView topLeftCell="A63" workbookViewId="0">
       <selection activeCell="C90" sqref="C90:C99"/>
     </sheetView>
   </sheetViews>
@@ -2090,7 +2113,7 @@
   <dimension ref="A1:B11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -2166,7 +2189,7 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Random</t>
+          <t>Mixed vocabulary</t>
         </is>
       </c>
     </row>
@@ -2221,10 +2244,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I11"/>
+  <dimension ref="A1:I13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G23" sqref="G23"/>
+      <selection activeCell="A13" sqref="A13:B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16"/>
@@ -2240,47 +2263,47 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="9" t="inlineStr">
+      <c r="A1" s="10" t="inlineStr">
         <is>
           <t>test_id</t>
         </is>
       </c>
-      <c r="B1" s="9" t="inlineStr">
+      <c r="B1" s="10" t="inlineStr">
         <is>
           <t>user_name</t>
         </is>
       </c>
-      <c r="C1" s="9" t="inlineStr">
+      <c r="C1" s="10" t="inlineStr">
         <is>
           <t>test_date_time</t>
         </is>
       </c>
-      <c r="D1" s="9" t="inlineStr">
+      <c r="D1" s="10" t="inlineStr">
         <is>
           <t>test_version</t>
         </is>
       </c>
-      <c r="E1" s="9" t="inlineStr">
+      <c r="E1" s="10" t="inlineStr">
         <is>
           <t>test_time_limit_sek</t>
         </is>
       </c>
-      <c r="F1" s="9" t="inlineStr">
+      <c r="F1" s="10" t="inlineStr">
         <is>
           <t>test_duration_sek</t>
         </is>
       </c>
-      <c r="G1" s="9" t="inlineStr">
+      <c r="G1" s="10" t="inlineStr">
         <is>
           <t>test_result_points</t>
         </is>
       </c>
-      <c r="H1" s="9" t="inlineStr">
+      <c r="H1" s="10" t="inlineStr">
         <is>
           <t>test_result_percentage</t>
         </is>
       </c>
-      <c r="I1" s="9" t="inlineStr">
+      <c r="I1" s="10" t="inlineStr">
         <is>
           <t>category</t>
         </is>
@@ -2677,10 +2700,8 @@
       <c r="E11" t="n">
         <v>60</v>
       </c>
-      <c r="F11" t="inlineStr">
-        <is>
-          <t>257.32</t>
-        </is>
+      <c r="F11" t="n">
+        <v>257.32</v>
       </c>
       <c r="G11" t="inlineStr">
         <is>
@@ -2693,6 +2714,90 @@
         </is>
       </c>
       <c r="I11" t="inlineStr">
+        <is>
+          <t>Processors</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="n">
+        <v>11</v>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>tomek</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>23-01-202517:54:15</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>PL-&gt;EN</t>
+        </is>
+      </c>
+      <c r="E12" t="n">
+        <v>300</v>
+      </c>
+      <c r="F12" t="n">
+        <v>127.32</v>
+      </c>
+      <c r="G12" t="inlineStr">
+        <is>
+          <t>(0/10)</t>
+        </is>
+      </c>
+      <c r="H12" t="inlineStr">
+        <is>
+          <t>0.00%</t>
+        </is>
+      </c>
+      <c r="I12" t="inlineStr">
+        <is>
+          <t>Random</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="n">
+        <v>12</v>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>Filip</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>31-01-2025 22:48:08</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>EN-&gt;PL</t>
+        </is>
+      </c>
+      <c r="E13" t="n">
+        <v>120</v>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>13.97</t>
+        </is>
+      </c>
+      <c r="G13" t="inlineStr">
+        <is>
+          <t>(2/2)</t>
+        </is>
+      </c>
+      <c r="H13" t="inlineStr">
+        <is>
+          <t>100.00%</t>
+        </is>
+      </c>
+      <c r="I13" t="inlineStr">
         <is>
           <t>Processors</t>
         </is>

</xml_diff>

<commit_message>
add comments in file manager
</commit_message>
<xml_diff>
--- a/test_database/tester_database.xlsx
+++ b/test_database/tester_database.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="0" yWindow="780" windowWidth="34200" windowHeight="19700" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="0" yWindow="780" windowWidth="34200" windowHeight="19700" tabRatio="600" firstSheet="0" activeTab="1" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="vocabulary" sheetId="1" state="visible" r:id="rId1"/>
@@ -555,9 +555,9 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C106"/>
+  <dimension ref="A1:C99"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A63" workbookViewId="0">
+    <sheetView topLeftCell="A63" workbookViewId="0">
       <selection activeCell="C106" sqref="A100:C106"/>
     </sheetView>
   </sheetViews>
@@ -568,17 +568,17 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="10" t="inlineStr">
+      <c r="A1" s="9" t="inlineStr">
         <is>
           <t>EN</t>
         </is>
       </c>
-      <c r="B1" s="10" t="inlineStr">
+      <c r="B1" s="9" t="inlineStr">
         <is>
           <t>PL</t>
         </is>
       </c>
-      <c r="C1" s="10" t="inlineStr">
+      <c r="C1" s="9" t="inlineStr">
         <is>
           <t>category</t>
         </is>
@@ -2052,111 +2052,6 @@
       </c>
       <c r="C99" t="n">
         <v>7</v>
-      </c>
-    </row>
-    <row r="100">
-      <c r="A100" t="inlineStr">
-        <is>
-          <t>screen</t>
-        </is>
-      </c>
-      <c r="B100" t="inlineStr">
-        <is>
-          <t>ekran</t>
-        </is>
-      </c>
-      <c r="C100" t="n">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="101">
-      <c r="A101" t="inlineStr">
-        <is>
-          <t>asdfasdf</t>
-        </is>
-      </c>
-      <c r="B101" t="inlineStr">
-        <is>
-          <t>polish</t>
-        </is>
-      </c>
-      <c r="C101" t="n">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="102">
-      <c r="A102" t="inlineStr">
-        <is>
-          <t>phone</t>
-        </is>
-      </c>
-      <c r="B102" t="inlineStr">
-        <is>
-          <t>telefon</t>
-        </is>
-      </c>
-      <c r="C102" t="n">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="103">
-      <c r="A103" t="inlineStr">
-        <is>
-          <t>dial</t>
-        </is>
-      </c>
-      <c r="B103" t="inlineStr">
-        <is>
-          <t>polacz</t>
-        </is>
-      </c>
-      <c r="C103" t="n">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="104">
-      <c r="A104" t="inlineStr">
-        <is>
-          <t>asdfasd</t>
-        </is>
-      </c>
-      <c r="B104" t="inlineStr">
-        <is>
-          <t>dfghdfgh</t>
-        </is>
-      </c>
-      <c r="C104" t="n">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="105">
-      <c r="A105" t="inlineStr">
-        <is>
-          <t>qwerwr</t>
-        </is>
-      </c>
-      <c r="B105" t="inlineStr">
-        <is>
-          <t>tyuityu</t>
-        </is>
-      </c>
-      <c r="C105" t="n">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="106">
-      <c r="A106" t="inlineStr">
-        <is>
-          <t>asdd</t>
-        </is>
-      </c>
-      <c r="B106" t="inlineStr">
-        <is>
-          <t>sgsdfg</t>
-        </is>
-      </c>
-      <c r="C106" t="n">
-        <v>11</v>
       </c>
     </row>
   </sheetData>
@@ -2170,10 +2065,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B12"/>
+  <dimension ref="A1:B8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B11" sqref="A9:B11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B12" sqref="A9:B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -2182,12 +2077,12 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="10" t="inlineStr">
+      <c r="A1" s="9" t="inlineStr">
         <is>
           <t>category_id</t>
         </is>
       </c>
-      <c r="B1" s="10" t="inlineStr">
+      <c r="B1" s="9" t="inlineStr">
         <is>
           <t>category_name</t>
         </is>
@@ -2260,46 +2155,6 @@
       <c r="B8" s="4" t="inlineStr">
         <is>
           <t>Law</t>
-        </is>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="n">
-        <v>8</v>
-      </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>Monitory</t>
-        </is>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="n">
-        <v>9</v>
-      </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>Phone</t>
-        </is>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="n">
-        <v>10</v>
-      </c>
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>Blablabla</t>
-        </is>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="n">
-        <v>11</v>
-      </c>
-      <c r="B12" t="inlineStr">
-        <is>
-          <t>Ytuiiii</t>
         </is>
       </c>
     </row>
@@ -2314,7 +2169,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I15"/>
+  <dimension ref="A1:I16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A13" sqref="A13:B15"/>
@@ -2333,47 +2188,47 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="8" t="inlineStr">
+      <c r="A1" s="10" t="inlineStr">
         <is>
           <t>test_id</t>
         </is>
       </c>
-      <c r="B1" s="8" t="inlineStr">
+      <c r="B1" s="10" t="inlineStr">
         <is>
           <t>user_name</t>
         </is>
       </c>
-      <c r="C1" s="8" t="inlineStr">
+      <c r="C1" s="10" t="inlineStr">
         <is>
           <t>test_date_time</t>
         </is>
       </c>
-      <c r="D1" s="8" t="inlineStr">
+      <c r="D1" s="10" t="inlineStr">
         <is>
           <t>test_version</t>
         </is>
       </c>
-      <c r="E1" s="8" t="inlineStr">
+      <c r="E1" s="10" t="inlineStr">
         <is>
           <t>test_time_limit_sek</t>
         </is>
       </c>
-      <c r="F1" s="8" t="inlineStr">
+      <c r="F1" s="10" t="inlineStr">
         <is>
           <t>test_duration_sek</t>
         </is>
       </c>
-      <c r="G1" s="8" t="inlineStr">
+      <c r="G1" s="10" t="inlineStr">
         <is>
           <t>test_result_points</t>
         </is>
       </c>
-      <c r="H1" s="8" t="inlineStr">
+      <c r="H1" s="10" t="inlineStr">
         <is>
           <t>test_result_percentage</t>
         </is>
       </c>
-      <c r="I1" s="8" t="inlineStr">
+      <c r="I1" s="10" t="inlineStr">
         <is>
           <t>category</t>
         </is>
@@ -2934,10 +2789,8 @@
       <c r="E15" t="n">
         <v>120</v>
       </c>
-      <c r="F15" t="inlineStr">
-        <is>
-          <t>7.62</t>
-        </is>
+      <c r="F15" t="n">
+        <v>7.62</v>
       </c>
       <c r="G15" t="inlineStr">
         <is>
@@ -2952,6 +2805,49 @@
       <c r="I15" t="inlineStr">
         <is>
           <t>Games Remastering</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="n">
+        <v>15</v>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>filip</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>02-02-2025 13:08:52</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>PL-&gt;EN</t>
+        </is>
+      </c>
+      <c r="E16" t="n">
+        <v>60</v>
+      </c>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>127.13</t>
+        </is>
+      </c>
+      <c r="G16" t="inlineStr">
+        <is>
+          <t>(6/30)</t>
+        </is>
+      </c>
+      <c r="H16" t="inlineStr">
+        <is>
+          <t>20.00%</t>
+        </is>
+      </c>
+      <c r="I16" t="inlineStr">
+        <is>
+          <t>Games Remastering, Processors, Graphic cards</t>
         </is>
       </c>
     </row>

</xml_diff>